<commit_message>
Todos los datasests generan en Gold su dataset enriquecido con el catálogo de artistas.
</commit_message>
<xml_diff>
--- a/datalake/bronze/artists_catalogue/artists_catalogue.xlsx
+++ b/datalake/bronze/artists_catalogue/artists_catalogue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Desktop\TFM\tfm_alvaro\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Desktop\TFM\tfm_alvaro\datalake\bronze\artists_catalogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{560DCBC0-BCD6-4C96-BAD6-D3AE54A8912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF82E27-A469-4794-809B-344D7FEE9808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53D4F322-FC8F-4374-991E-81A179F8E64B}"/>
   </bookViews>
@@ -642,16 +642,16 @@
     <t>Artista</t>
   </si>
   <si>
-    <t>Año nacimiento</t>
-  </si>
-  <si>
-    <t>Año muerte</t>
-  </si>
-  <si>
     <t>Christo Vladimirov Javacheff</t>
   </si>
   <si>
     <t>Jeanne-Claude Denat de Guillebon</t>
+  </si>
+  <si>
+    <t>AñoNacimiento</t>
+  </si>
+  <si>
+    <t>AñoMuerte</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,10 +1025,10 @@
         <v>201</v>
       </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>163</v>
       </c>
       <c r="B167" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C167">
         <v>1935</v>
@@ -3306,7 +3306,7 @@
         <v>163</v>
       </c>
       <c r="B168" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C168">
         <v>1935</v>

</xml_diff>